<commit_message>
Updated CHE_grids model - 2025-08-14 22:00
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE_grids/SuppXLS/scen_tsparameters_triple_1.xlsx
+++ b/VerveStacks_CHE_grids/SuppXLS/scen_tsparameters_triple_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3902F7A-21D2-4526-A7E0-0E9465CECFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E59523-3A00-42BE-9CF6-CBF341690779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -1074,10 +1074,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S1aH3,S1b0205h08,S1b0205h10,S2c0415h14,S4aH2,S1aH5,S1b0205h09,S1b0205h14,S1b0205h15,S2aH4,S2aH5,S2c0415h08,S5aH2,S5aH5,S6aH2,S2c0415h07,S2c0415h13,S2c0415h15,S1b0205h12,S2c0415h09,S2c0415h11,S3aH7,S1b0205h13,S2d0427h13,S4aH5,S2d0427h07,S2d0427h10,S2d0427h17,S6aH5,S1b0205h18,S2aH7,S2d0427h08,S3aH4,S4aH3,S4aH4,S1aH2,S1aH7,S1b0205h11,S2aH3,S2d0427h18,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S1aH6,S2c0415h12,S2c0415h17,S2d0427h11,S6aH7,S3aH2,S1b0205h16,S2aH6,S2d0427h09,S3aH5,S5aH3,S1b0205h07,S2c0415h10,S2c0415h16,S2c0415h18,S2d0427h12,S3aH3,S1aH4,S2aH2,S2d0427h15,S4aH6,S1b0205h17,S2d0427h14,S2d0427h16,S5aH4,S6aH3,S6aH4</t>
+    <t>S1b0205h07,S2c0415h10,S2c0415h16,S2c0415h18,S2d0427h12,S3aH3,S2c0415h17,S2d0427h11,S6aH7,S1aH3,S1aH2,S1aH7,S1b0205h11,S2aH3,S2d0427h18,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S1aH5,S1b0205h09,S1b0205h14,S1b0205h15,S2aH4,S2aH5,S2c0415h08,S5aH2,S5aH5,S6aH2,S1b0205h12,S2c0415h09,S2c0415h11,S3aH7,S1aH4,S2aH2,S2d0427h15,S4aH6,S1b0205h13,S2d0427h13,S4aH5,S1b0205h17,S2d0427h14,S2d0427h16,S5aH4,S6aH3,S6aH4,S1aH6,S2c0415h12,S1b0205h16,S2aH6,S2d0427h09,S3aH5,S5aH3,S1b0205h08,S1b0205h10,S2c0415h14,S4aH2,S3aH2,S2d0427h07,S2d0427h10,S2d0427h17,S6aH5,S2c0415h07,S2c0415h13,S2c0415h15,S1b0205h18,S2aH7,S2d0427h08,S3aH4,S4aH3,S4aH4</t>
   </si>
   <si>
-    <t>S1b0205h05,S1b0205h19,S2aH1,S2c0415h01,S5aH8,S2c0415h20,S1aH1,S1b0205h04,S2aH8,S2d0427h20,S1b0205h01,S1b0205h20,S2c0415h03,S2c0415h05,S2c0415h24,S2c0415h21,S4aH8,S1b0205h02,S2d0427h01,S2d0427h19,S1b0205h24,S2c0415h22,S2d0427h05,S2d0427h22,S2c0415h23,S6aH8,S1b0205h06,S1b0205h21,S2c0415h02,S2c0415h19,S2d0427h03,S3aH1,S3aH8,S1aH8,S1b0205h22,S2d0427h02,S2d0427h06,S2d0427h23,S5aH1,S1b0205h23,S2c0415h06,S2d0427h04,S2d0427h24,S2c0415h04,S2d0427h21,S4aH1,S6aH1,S1b0205h03</t>
+    <t>S1b0205h23,S2c0415h06,S2d0427h04,S2d0427h24,S1b0205h06,S1b0205h21,S2c0415h02,S2c0415h19,S2d0427h03,S3aH1,S1b0205h05,S1b0205h24,S2c0415h22,S2d0427h05,S2d0427h22,S2c0415h20,S2aH8,S2d0427h20,S2c0415h04,S2d0427h21,S4aH1,S6aH1,S1b0205h01,S1b0205h20,S2c0415h03,S2c0415h05,S2c0415h24,S1b0205h03,S2c0415h23,S6aH8,S1aH8,S1b0205h22,S2d0427h02,S2d0427h06,S2d0427h23,S5aH1,S1b0205h19,S2aH1,S2c0415h01,S5aH8,S3aH8,S2c0415h21,S4aH8,S1aH1,S1b0205h04,S1b0205h02,S2d0427h01,S2d0427h19</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S1b0205h05,S1b0205h19,S2aH1,S2c0415h01,S5aH8,S2c0415h20,S1aH1,S1b0205h04,S2aH8,S2d0427h20,S1b0205h01,S1b0205h20,S2c0415h03,S2c0415h05,S2c0415h24,S2c0415h21,S4aH8,S1b0205h02,S2d0427h01,S2d0427h19,S1b0205h24,S2c0415h22,S2d0427h05,S2d0427h22,S2c0415h23,S6aH8,S1b0205h06,S1b0205h21,S2c0415h02,S2c0415h19,S2d0427h03,S3aH1,S3aH8,S1aH8,S1b0205h22,S2d0427h02,S2d0427h06,S2d0427h23,S5aH1,S1b0205h23,S2c0415h06,S2d0427h04,S2d0427h24,S2c0415h04,S2d0427h21,S4aH1,S6aH1,S1b0205h03</v>
+        <v>S1b0205h23,S2c0415h06,S2d0427h04,S2d0427h24,S1b0205h06,S1b0205h21,S2c0415h02,S2c0415h19,S2d0427h03,S3aH1,S1b0205h05,S1b0205h24,S2c0415h22,S2d0427h05,S2d0427h22,S2c0415h20,S2aH8,S2d0427h20,S2c0415h04,S2d0427h21,S4aH1,S6aH1,S1b0205h01,S1b0205h20,S2c0415h03,S2c0415h05,S2c0415h24,S1b0205h03,S2c0415h23,S6aH8,S1aH8,S1b0205h22,S2d0427h02,S2d0427h06,S2d0427h23,S5aH1,S1b0205h19,S2aH1,S2c0415h01,S5aH8,S3aH8,S2c0415h21,S4aH8,S1aH1,S1b0205h04,S1b0205h02,S2d0427h01,S2d0427h19</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S1aH3,S1b0205h08,S1b0205h10,S2c0415h14,S4aH2,S1aH5,S1b0205h09,S1b0205h14,S1b0205h15,S2aH4,S2aH5,S2c0415h08,S5aH2,S5aH5,S6aH2,S2c0415h07,S2c0415h13,S2c0415h15,S1b0205h12,S2c0415h09,S2c0415h11,S3aH7,S1b0205h13,S2d0427h13,S4aH5,S2d0427h07,S2d0427h10,S2d0427h17,S6aH5,S1b0205h18,S2aH7,S2d0427h08,S3aH4,S4aH3,S4aH4,S1aH2,S1aH7,S1b0205h11,S2aH3,S2d0427h18,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S1aH6,S2c0415h12,S2c0415h17,S2d0427h11,S6aH7,S3aH2,S1b0205h16,S2aH6,S2d0427h09,S3aH5,S5aH3,S1b0205h07,S2c0415h10,S2c0415h16,S2c0415h18,S2d0427h12,S3aH3,S1aH4,S2aH2,S2d0427h15,S4aH6,S1b0205h17,S2d0427h14,S2d0427h16,S5aH4,S6aH3,S6aH4</v>
+        <v>S1b0205h07,S2c0415h10,S2c0415h16,S2c0415h18,S2d0427h12,S3aH3,S2c0415h17,S2d0427h11,S6aH7,S1aH3,S1aH2,S1aH7,S1b0205h11,S2aH3,S2d0427h18,S3aH6,S4aH7,S5aH6,S5aH7,S6aH6,S1aH5,S1b0205h09,S1b0205h14,S1b0205h15,S2aH4,S2aH5,S2c0415h08,S5aH2,S5aH5,S6aH2,S1b0205h12,S2c0415h09,S2c0415h11,S3aH7,S1aH4,S2aH2,S2d0427h15,S4aH6,S1b0205h13,S2d0427h13,S4aH5,S1b0205h17,S2d0427h14,S2d0427h16,S5aH4,S6aH3,S6aH4,S1aH6,S2c0415h12,S1b0205h16,S2aH6,S2d0427h09,S3aH5,S5aH3,S1b0205h08,S1b0205h10,S2c0415h14,S4aH2,S3aH2,S2d0427h07,S2d0427h10,S2d0427h17,S6aH5,S2c0415h07,S2c0415h13,S2c0415h15,S1b0205h18,S2aH7,S2d0427h08,S3aH4,S4aH3,S4aH4</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2293,7 +2293,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317C997A-8543-4341-A862-AC7926E61BD4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F686053-E29F-4BEB-8FF9-A6892FBF8097}">
   <dimension ref="B2:F83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3010,7 +3010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7568E128-575E-4607-A5A6-B517AB942794}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51FB3113-D11C-4FA8-A458-1C70013173A3}">
   <dimension ref="B2:O3123"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3089,10 +3089,10 @@
         <v>317</v>
       </c>
       <c r="M4" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="N4">
-        <v>8.0605632899210883E-2</v>
+        <v>0.17653172515557836</v>
       </c>
       <c r="O4" t="s">
         <v>351</v>
@@ -3159,10 +3159,10 @@
         <v>317</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="N6">
-        <v>0.26179508564829657</v>
+        <v>0.40660807082825429</v>
       </c>
       <c r="O6" t="s">
         <v>351</v>
@@ -3194,10 +3194,10 @@
         <v>317</v>
       </c>
       <c r="M7" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="N7">
-        <v>0.40660807082825429</v>
+        <v>7.9527811637903387E-2</v>
       </c>
       <c r="O7" t="s">
         <v>351</v>
@@ -3229,10 +3229,10 @@
         <v>317</v>
       </c>
       <c r="M8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N8">
-        <v>7.9527811637903387E-2</v>
+        <v>0.26179508564829657</v>
       </c>
       <c r="O8" t="s">
         <v>351</v>
@@ -3264,10 +3264,10 @@
         <v>317</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="N9">
-        <v>0.17653172515557836</v>
+        <v>8.0605632899210883E-2</v>
       </c>
       <c r="O9" t="s">
         <v>351</v>
@@ -81363,7 +81363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76B3E98-3FFF-4199-9671-A0E90C7F9040}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1DBB5B-BF26-41E5-A7BE-B04D73E4ACB2}">
   <dimension ref="B2:O243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>